<commit_message>
editing the diagram of the 20th and the expected output
</commit_message>
<xml_diff>
--- a/expected_output.xlsx
+++ b/expected_output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DMontecino/Documents/WH_DATABASE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA83AA63-C448-0544-957F-D17323D6172F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A487EE3-2D63-4E41-9BDB-68A8A2D8A780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15420" yWindow="1800" windowWidth="35840" windowHeight="20920" xr2:uid="{6A3CFA6F-5662-0044-8A80-3174EF898E1D}"/>
+    <workbookView xWindow="0" yWindow="1480" windowWidth="35840" windowHeight="20920" xr2:uid="{6A3CFA6F-5662-0044-8A80-3174EF898E1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,6 +58,9 @@
     <author>tc={8C164F4C-D6E2-7041-9565-5D8D6BF5F673}</author>
     <author>tc={F31A5A15-60CE-E247-96FC-962343518F52}</author>
     <author>tc={EA11F198-6E72-2342-9968-208B515C022C}</author>
+    <author>tc={7ED93411-5379-2347-BC90-090F2D80C4B7}</author>
+    <author>tc={73D77EFC-4F8F-CE49-9CE4-E0B88F6E328F}</author>
+    <author>tc={703B8DCF-08FF-A44D-BAEC-11A8932259C3}</author>
     <author>tc={07CF1E39-8A73-D04F-B674-B2A056169D6F}</author>
     <author>tc={9F856851-F726-054E-B8FE-D6434E5D151C}</author>
     <author>tc={BC1252D4-D567-1448-9913-0C1081A0F563}</author>
@@ -251,7 +254,31 @@
     For observations is always 1. 1 observation source has 1 record . No more, no less. How many records has any source provided?</t>
       </text>
     </comment>
-    <comment ref="BN2" authorId="20" shapeId="0" xr:uid="{07CF1E39-8A73-D04F-B674-B2A056169D6F}">
+    <comment ref="BK2" authorId="20" shapeId="0" xr:uid="{7ED93411-5379-2347-BC90-090F2D80C4B7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Apply to animal and observation sources. Only one option for the former and several options for he latter</t>
+      </text>
+    </comment>
+    <comment ref="BL2" authorId="21" shapeId="0" xr:uid="{73D77EFC-4F8F-CE49-9CE4-E0B88F6E328F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Several options. Does apply to obs and animal sources only.</t>
+      </text>
+    </comment>
+    <comment ref="BM2" authorId="22" shapeId="0" xr:uid="{703B8DCF-08FF-A44D-BAEC-11A8932259C3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Only for obsevration and animal sources</t>
+      </text>
+    </comment>
+    <comment ref="BN2" authorId="23" shapeId="0" xr:uid="{07CF1E39-8A73-D04F-B674-B2A056169D6F}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -259,7 +286,7 @@
     For observations and animals only. In both cases, each source can have many causes of injury and diseases </t>
       </text>
     </comment>
-    <comment ref="BO2" authorId="21" shapeId="0" xr:uid="{9F856851-F726-054E-B8FE-D6434E5D151C}">
+    <comment ref="BO2" authorId="24" shapeId="0" xr:uid="{9F856851-F726-054E-B8FE-D6434E5D151C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -267,7 +294,7 @@
     Just like in previous column</t>
       </text>
     </comment>
-    <comment ref="CC2" authorId="22" shapeId="0" xr:uid="{BC1252D4-D567-1448-9913-0C1081A0F563}">
+    <comment ref="CC2" authorId="25" shapeId="0" xr:uid="{BC1252D4-D567-1448-9913-0C1081A0F563}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -275,7 +302,7 @@
     Applies only for inv source records</t>
       </text>
     </comment>
-    <comment ref="CD2" authorId="23" shapeId="0" xr:uid="{2820BBED-4EE7-4548-834F-726AB3B48E0E}">
+    <comment ref="CD2" authorId="26" shapeId="0" xr:uid="{2820BBED-4EE7-4548-834F-726AB3B48E0E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -283,7 +310,7 @@
     As previous comment</t>
       </text>
     </comment>
-    <comment ref="CE2" authorId="24" shapeId="0" xr:uid="{51EE57F4-5350-864E-A80C-CA118CEFCF8C}">
+    <comment ref="CE2" authorId="27" shapeId="0" xr:uid="{51EE57F4-5350-864E-A80C-CA118CEFCF8C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -291,7 +318,7 @@
     Does not apply for observations</t>
       </text>
     </comment>
-    <comment ref="CF2" authorId="25" shapeId="0" xr:uid="{862605B5-09DC-0D43-A0CB-99B0BED07F1D}">
+    <comment ref="CF2" authorId="28" shapeId="0" xr:uid="{862605B5-09DC-0D43-A0CB-99B0BED07F1D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -299,7 +326,7 @@
     These are tags to group sources below the incident (below the lat Lon), It is a single option for each source record</t>
       </text>
     </comment>
-    <comment ref="AV3" authorId="26" shapeId="0" xr:uid="{6EA9A32C-4E71-2543-B874-318BA7BC8F28}">
+    <comment ref="AV3" authorId="29" shapeId="0" xr:uid="{6EA9A32C-4E71-2543-B874-318BA7BC8F28}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -307,7 +334,7 @@
     For each obs, animal, and env source only one species is possible. For inv species, several are possible</t>
       </text>
     </comment>
-    <comment ref="BK3" authorId="27" shapeId="0" xr:uid="{20381252-538A-3349-A73F-60A29DB73880}">
+    <comment ref="BK3" authorId="30" shapeId="0" xr:uid="{20381252-538A-3349-A73F-60A29DB73880}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -315,7 +342,7 @@
     2 cats of captivity for the same observed species</t>
       </text>
     </comment>
-    <comment ref="BL3" authorId="28" shapeId="0" xr:uid="{5298E563-C6AE-1B42-8909-D5C50E574F99}">
+    <comment ref="BL3" authorId="31" shapeId="0" xr:uid="{5298E563-C6AE-1B42-8909-D5C50E574F99}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -323,7 +350,7 @@
     Two anomalies in each group of animals per captivity category</t>
       </text>
     </comment>
-    <comment ref="BN3" authorId="29" shapeId="0" xr:uid="{FE6AB3F1-9970-B246-86D6-C824649A558E}">
+    <comment ref="BN3" authorId="32" shapeId="0" xr:uid="{FE6AB3F1-9970-B246-86D6-C824649A558E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -331,7 +358,7 @@
     There could be many but in this example only one cause for the species in bot. Captivity categories</t>
       </text>
     </comment>
-    <comment ref="BO3" authorId="30" shapeId="0" xr:uid="{88517524-4EEF-2D42-96AA-4BE0D8D990C6}">
+    <comment ref="BO3" authorId="33" shapeId="0" xr:uid="{88517524-4EEF-2D42-96AA-4BE0D8D990C6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -339,7 +366,7 @@
     In the example only a single cause of death but it can be multiple per species per category of captivity</t>
       </text>
     </comment>
-    <comment ref="BG8" authorId="31" shapeId="0" xr:uid="{4962E53F-0802-9E4D-B3DB-33B6A515B08A}">
+    <comment ref="BG8" authorId="34" shapeId="0" xr:uid="{4962E53F-0802-9E4D-B3DB-33B6A515B08A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -347,7 +374,7 @@
     Same individual different record</t>
       </text>
     </comment>
-    <comment ref="BN8" authorId="32" shapeId="0" xr:uid="{B1CDC667-B90E-6F4D-9EDC-C9C8943D2BBC}">
+    <comment ref="BN8" authorId="35" shapeId="0" xr:uid="{B1CDC667-B90E-6F4D-9EDC-C9C8943D2BBC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -355,7 +382,7 @@
     Same animal has 2 causes of death</t>
       </text>
     </comment>
-    <comment ref="BO8" authorId="33" shapeId="0" xr:uid="{050447EF-E556-7449-9060-23A1CE1DD75B}">
+    <comment ref="BO8" authorId="36" shapeId="0" xr:uid="{050447EF-E556-7449-9060-23A1CE1DD75B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -363,7 +390,7 @@
     The animal could have multiple reasons to have died but in the example it did not die</t>
       </text>
     </comment>
-    <comment ref="BG9" authorId="34" shapeId="0" xr:uid="{B39A306D-1265-D445-9CF2-D0F8BDAEE66C}">
+    <comment ref="BG9" authorId="37" shapeId="0" xr:uid="{B39A306D-1265-D445-9CF2-D0F8BDAEE66C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -371,7 +398,7 @@
     The second record of this female used in 3 surveillance objectives</t>
       </text>
     </comment>
-    <comment ref="BH9" authorId="35" shapeId="0" xr:uid="{0C1D1F54-BE5E-A44C-9073-18BDE983E0D7}">
+    <comment ref="BH9" authorId="38" shapeId="0" xr:uid="{0C1D1F54-BE5E-A44C-9073-18BDE983E0D7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -379,7 +406,7 @@
     Second record of the female. The first record was taken in location 1. See the previous cell</t>
       </text>
     </comment>
-    <comment ref="BN9" authorId="36" shapeId="0" xr:uid="{627FC601-D173-C94C-A986-CD44A5302850}">
+    <comment ref="BN9" authorId="39" shapeId="0" xr:uid="{627FC601-D173-C94C-A986-CD44A5302850}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -387,7 +414,7 @@
     Same animal has 2 causes of death</t>
       </text>
     </comment>
-    <comment ref="BO9" authorId="37" shapeId="0" xr:uid="{0E542CDE-0A3E-7040-B349-85124BE442DD}">
+    <comment ref="BO9" authorId="40" shapeId="0" xr:uid="{0E542CDE-0A3E-7040-B349-85124BE442DD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -395,7 +422,7 @@
     The animal could have multiple reasons to have died but in the example it did not die</t>
       </text>
     </comment>
-    <comment ref="BN11" authorId="38" shapeId="0" xr:uid="{C9CEE0D6-A721-0A4A-90E9-C69B77CF5041}">
+    <comment ref="BN11" authorId="41" shapeId="0" xr:uid="{C9CEE0D6-A721-0A4A-90E9-C69B77CF5041}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -403,7 +430,7 @@
     Same animal has 2 causes of death</t>
       </text>
     </comment>
-    <comment ref="BN13" authorId="39" shapeId="0" xr:uid="{493486A8-442A-4847-8A2D-623A8F3C8682}">
+    <comment ref="BN13" authorId="42" shapeId="0" xr:uid="{493486A8-442A-4847-8A2D-623A8F3C8682}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -411,7 +438,7 @@
     Same animal has 2 causes of death</t>
       </text>
     </comment>
-    <comment ref="BG15" authorId="40" shapeId="0" xr:uid="{4D334DF3-0BED-3344-96BC-7C3FFCFF2A04}">
+    <comment ref="BG15" authorId="43" shapeId="0" xr:uid="{4D334DF3-0BED-3344-96BC-7C3FFCFF2A04}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -419,7 +446,7 @@
     This is the second record of this env source. The previous record could have been in FA1</t>
       </text>
     </comment>
-    <comment ref="BH15" authorId="41" shapeId="0" xr:uid="{EF3CC71D-14E3-9043-B4CA-A07BAD4B54E9}">
+    <comment ref="BH15" authorId="44" shapeId="0" xr:uid="{EF3CC71D-14E3-9043-B4CA-A07BAD4B54E9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -427,7 +454,7 @@
     For env sources the Source is the actual place of collection. From S4, 2 records have been made. The previous record could have been in FA1</t>
       </text>
     </comment>
-    <comment ref="BK15" authorId="42" shapeId="0" xr:uid="{0FDEC139-B49D-B844-8C5F-F8EF42933E1C}">
+    <comment ref="BK15" authorId="45" shapeId="0" xr:uid="{0FDEC139-B49D-B844-8C5F-F8EF42933E1C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -435,7 +462,7 @@
     Invertebrate and environmental sources do not have anomalies or captivity categories</t>
       </text>
     </comment>
-    <comment ref="AV16" authorId="43" shapeId="0" xr:uid="{1E62C786-C23F-6748-A1C8-D55C26F6169E}">
+    <comment ref="AV16" authorId="46" shapeId="0" xr:uid="{1E62C786-C23F-6748-A1C8-D55C26F6169E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -443,7 +470,7 @@
     Several species can apply for Invertebrates Sources</t>
       </text>
     </comment>
-    <comment ref="BG16" authorId="44" shapeId="0" xr:uid="{0424A52E-E57A-B144-8412-DFB671388F8C}">
+    <comment ref="BG16" authorId="47" shapeId="0" xr:uid="{0424A52E-E57A-B144-8412-DFB671388F8C}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1223,7 +1250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1231,19 +1258,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1261,64 +1279,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1326,12 +1305,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1343,6 +1316,27 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1733,6 +1727,15 @@
   <threadedComment ref="BH2" dT="2023-06-22T16:51:22.31" personId="{FA2B6155-3D78-AE49-8982-BCF98E38F70E}" id="{EA11F198-6E72-2342-9968-208B515C022C}">
     <text>For observations is always 1. 1 observation source has 1 record . No more, no less. How many records has any source provided?</text>
   </threadedComment>
+  <threadedComment ref="BK2" dT="2023-06-29T23:36:42.34" personId="{FA2B6155-3D78-AE49-8982-BCF98E38F70E}" id="{7ED93411-5379-2347-BC90-090F2D80C4B7}">
+    <text>Apply to animal and observation sources. Only one option for the former and several options for he latter</text>
+  </threadedComment>
+  <threadedComment ref="BL2" dT="2023-06-29T23:37:20.76" personId="{FA2B6155-3D78-AE49-8982-BCF98E38F70E}" id="{73D77EFC-4F8F-CE49-9CE4-E0B88F6E328F}">
+    <text>Several options. Does apply to obs and animal sources only.</text>
+  </threadedComment>
+  <threadedComment ref="BM2" dT="2023-06-29T23:38:31.83" personId="{FA2B6155-3D78-AE49-8982-BCF98E38F70E}" id="{703B8DCF-08FF-A44D-BAEC-11A8932259C3}">
+    <text>Only for obsevration and animal sources</text>
+  </threadedComment>
   <threadedComment ref="BN2" dT="2023-06-22T15:58:29.29" personId="{FA2B6155-3D78-AE49-8982-BCF98E38F70E}" id="{07CF1E39-8A73-D04F-B674-B2A056169D6F}">
     <text xml:space="preserve">For observations and animals only. In both cases, each source can have many causes of injury and diseases </text>
   </threadedComment>
@@ -1815,8 +1818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE705D81-1BE1-C443-B6B1-40DF90B96FA9}">
   <dimension ref="A1:DW23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DT1" zoomScale="40" workbookViewId="0">
-      <selection activeCell="DS8" sqref="DS8"/>
+    <sheetView tabSelected="1" topLeftCell="BL1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="BP10" sqref="BP10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1863,16 +1866,16 @@
     <col min="46" max="46" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="26.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="26.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="50" max="51" width="30" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="17.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="17.5" style="6" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="28" style="9" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="28" style="9" customWidth="1"/>
-    <col min="57" max="57" width="15.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="19.1640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="26" style="13" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="28" style="6" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="28" style="6" customWidth="1"/>
+    <col min="57" max="57" width="15.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="19.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="22.83203125" style="1" customWidth="1"/>
     <col min="61" max="61" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="21" style="1" bestFit="1" customWidth="1"/>
@@ -1882,7 +1885,7 @@
     <col min="66" max="66" width="36.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="30" style="1" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="29.1640625" style="9" customWidth="1"/>
+    <col min="69" max="69" width="29.1640625" style="6" customWidth="1"/>
     <col min="70" max="70" width="36" style="1" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="34.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -1891,13 +1894,13 @@
     <col min="75" max="75" width="29.5" style="1" bestFit="1" customWidth="1"/>
     <col min="76" max="76" width="35.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="43.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="43.5" style="9" customWidth="1"/>
-    <col min="79" max="80" width="43.5" style="13" customWidth="1"/>
-    <col min="81" max="81" width="29.1640625" style="17" customWidth="1"/>
-    <col min="82" max="82" width="40.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="29.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="43.5" style="6" customWidth="1"/>
+    <col min="79" max="80" width="43.5" style="1" customWidth="1"/>
+    <col min="81" max="81" width="29.1640625" style="6" customWidth="1"/>
+    <col min="82" max="82" width="40.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="29.1640625" style="6" bestFit="1" customWidth="1"/>
     <col min="84" max="88" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="24.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="24.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="91" max="91" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -1921,7 +1924,7 @@
     <col min="110" max="110" width="30" style="1" bestFit="1" customWidth="1"/>
     <col min="111" max="111" width="30" style="1" customWidth="1"/>
     <col min="112" max="112" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="31.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="31.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="114" max="114" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="115" max="115" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="116" max="116" width="53.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -1940,480 +1943,480 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:127" x14ac:dyDescent="0.2">
-      <c r="AW1" s="4" t="s">
+      <c r="AW1" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="AX1" s="4"/>
-      <c r="AY1" s="4"/>
-      <c r="AZ1" s="4" t="s">
+      <c r="AX1" s="28"/>
+      <c r="AY1" s="28"/>
+      <c r="AZ1" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="BA1" s="4"/>
-      <c r="BB1" s="4"/>
-      <c r="BC1" s="8" t="s">
+      <c r="BA1" s="28"/>
+      <c r="BB1" s="28"/>
+      <c r="BC1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="BD1" s="8" t="s">
+      <c r="BD1" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="31"/>
-      <c r="BG1" s="23" t="s">
+      <c r="BE1" s="15"/>
+      <c r="BF1" s="15"/>
+      <c r="BG1" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="BH1" s="28"/>
-      <c r="BI1" s="28"/>
-      <c r="BJ1" s="28"/>
-      <c r="BK1" s="28"/>
-      <c r="BL1" s="28"/>
-      <c r="BM1" s="28"/>
-      <c r="BN1" s="28"/>
-      <c r="BO1" s="28"/>
-      <c r="BP1" s="29"/>
-      <c r="BQ1" s="16" t="s">
+      <c r="BH1" s="26"/>
+      <c r="BI1" s="26"/>
+      <c r="BJ1" s="26"/>
+      <c r="BK1" s="26"/>
+      <c r="BL1" s="26"/>
+      <c r="BM1" s="26"/>
+      <c r="BN1" s="26"/>
+      <c r="BO1" s="26"/>
+      <c r="BP1" s="27"/>
+      <c r="BQ1" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="BR1" s="16"/>
-      <c r="BS1" s="16"/>
-      <c r="BT1" s="16"/>
-      <c r="BU1" s="16"/>
-      <c r="BV1" s="16"/>
-      <c r="BW1" s="16"/>
-      <c r="BX1" s="16"/>
-      <c r="BY1" s="16"/>
-      <c r="BZ1" s="16" t="s">
+      <c r="BR1" s="29"/>
+      <c r="BS1" s="29"/>
+      <c r="BT1" s="29"/>
+      <c r="BU1" s="29"/>
+      <c r="BV1" s="29"/>
+      <c r="BW1" s="29"/>
+      <c r="BX1" s="29"/>
+      <c r="BY1" s="29"/>
+      <c r="BZ1" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="CA1" s="16"/>
-      <c r="CB1" s="16"/>
-      <c r="CC1" s="16" t="s">
+      <c r="CA1" s="29"/>
+      <c r="CB1" s="29"/>
+      <c r="CC1" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="CD1" s="16"/>
-      <c r="CK1" s="24" t="s">
+      <c r="CD1" s="29"/>
+      <c r="CK1" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="CL1" s="25"/>
-      <c r="CM1" s="25"/>
-      <c r="CN1" s="25"/>
-      <c r="CO1" s="25"/>
-      <c r="CP1" s="25"/>
-      <c r="CQ1" s="25"/>
-      <c r="CR1" s="25"/>
-      <c r="CS1" s="25"/>
-      <c r="CT1" s="25"/>
-      <c r="CU1" s="25"/>
-      <c r="CV1" s="25"/>
-      <c r="CW1" s="25"/>
-      <c r="CX1" s="25"/>
-      <c r="CY1" s="25"/>
-      <c r="CZ1" s="25"/>
-      <c r="DA1" s="25"/>
-      <c r="DB1" s="25"/>
-      <c r="DC1" s="25"/>
-      <c r="DD1" s="25"/>
-      <c r="DE1" s="25"/>
-      <c r="DF1" s="25"/>
-      <c r="DG1" s="25"/>
-      <c r="DH1" s="25"/>
-      <c r="DI1" s="24" t="s">
+      <c r="CL1" s="24"/>
+      <c r="CM1" s="24"/>
+      <c r="CN1" s="24"/>
+      <c r="CO1" s="24"/>
+      <c r="CP1" s="24"/>
+      <c r="CQ1" s="24"/>
+      <c r="CR1" s="24"/>
+      <c r="CS1" s="24"/>
+      <c r="CT1" s="24"/>
+      <c r="CU1" s="24"/>
+      <c r="CV1" s="24"/>
+      <c r="CW1" s="24"/>
+      <c r="CX1" s="24"/>
+      <c r="CY1" s="24"/>
+      <c r="CZ1" s="24"/>
+      <c r="DA1" s="24"/>
+      <c r="DB1" s="24"/>
+      <c r="DC1" s="24"/>
+      <c r="DD1" s="24"/>
+      <c r="DE1" s="24"/>
+      <c r="DF1" s="24"/>
+      <c r="DG1" s="24"/>
+      <c r="DH1" s="24"/>
+      <c r="DI1" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="DJ1" s="25"/>
-      <c r="DK1" s="25"/>
-      <c r="DL1" s="25"/>
-      <c r="DM1" s="25"/>
-      <c r="DN1" s="25"/>
-      <c r="DO1" s="25"/>
-      <c r="DP1" s="25"/>
-      <c r="DQ1" s="25"/>
-      <c r="DR1" s="25"/>
-      <c r="DS1" s="25"/>
-      <c r="DT1" s="25"/>
-      <c r="DU1" s="25"/>
-      <c r="DV1" s="25"/>
-      <c r="DW1" s="25"/>
+      <c r="DJ1" s="24"/>
+      <c r="DK1" s="24"/>
+      <c r="DL1" s="24"/>
+      <c r="DM1" s="24"/>
+      <c r="DN1" s="24"/>
+      <c r="DO1" s="24"/>
+      <c r="DP1" s="24"/>
+      <c r="DQ1" s="24"/>
+      <c r="DR1" s="24"/>
+      <c r="DS1" s="24"/>
+      <c r="DT1" s="24"/>
+      <c r="DU1" s="24"/>
+      <c r="DV1" s="24"/>
+      <c r="DW1" s="24"/>
     </row>
-    <row r="2" spans="1:127" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:127" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="L2" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="P2" s="27" t="s">
+      <c r="P2" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="S2" s="33" t="s">
+      <c r="S2" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="T2" s="33" t="s">
+      <c r="T2" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="V2" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="W2" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="X2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Y2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="AA2" s="12" t="s">
+      <c r="AA2" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="AB2" s="12" t="s">
+      <c r="AB2" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="AC2" s="12" t="s">
+      <c r="AC2" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="AD2" s="27" t="s">
+      <c r="AD2" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AE2" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AF2" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AG2" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AH2" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="AI2" s="12" t="s">
+      <c r="AI2" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AK2" s="5" t="s">
+      <c r="AK2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AL2" s="34" t="s">
+      <c r="AL2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AM2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AN2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AO2" s="6" t="s">
+      <c r="AO2" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="AP2" s="7" t="s">
+      <c r="AP2" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="AQ2" s="7" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="AR2" s="5" t="s">
+      <c r="AR2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AS2" s="5" t="s">
+      <c r="AS2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AT2" s="6" t="s">
+      <c r="AT2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AU2" s="5" t="s">
+      <c r="AU2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AV2" s="5" t="s">
+      <c r="AV2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AW2" s="35" t="s">
+      <c r="AW2" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AX2" s="36" t="s">
+      <c r="AX2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AY2" s="36" t="s">
+      <c r="AY2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AZ2" s="35" t="s">
+      <c r="AZ2" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="BA2" s="36" t="s">
+      <c r="BA2" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="BB2" s="36" t="s">
+      <c r="BB2" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="BC2" s="35" t="s">
+      <c r="BC2" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="BD2" s="37" t="s">
+      <c r="BD2" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="BE2" s="32" t="s">
+      <c r="BE2" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="BF2" s="38" t="s">
+      <c r="BF2" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="BG2" s="21" t="s">
+      <c r="BG2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="BH2" s="27" t="s">
+      <c r="BH2" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="BI2" s="36" t="s">
+      <c r="BI2" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="BJ2" s="36" t="s">
+      <c r="BJ2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="BK2" s="5" t="s">
+      <c r="BK2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BL2" s="5" t="s">
+      <c r="BL2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="BM2" s="5" t="s">
+      <c r="BM2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="BN2" s="6" t="s">
+      <c r="BN2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="BO2" s="6" t="s">
+      <c r="BO2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="BP2" s="34" t="s">
+      <c r="BP2" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="BQ2" s="20" t="s">
+      <c r="BQ2" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="BR2" s="12" t="s">
+      <c r="BR2" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="BS2" s="12" t="s">
+      <c r="BS2" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="BT2" s="12" t="s">
+      <c r="BT2" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="BU2" s="12" t="s">
+      <c r="BU2" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="BV2" s="12" t="s">
+      <c r="BV2" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="BW2" s="12" t="s">
+      <c r="BW2" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="BX2" s="12" t="s">
+      <c r="BX2" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="BY2" s="12" t="s">
+      <c r="BY2" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="BZ2" s="20" t="s">
+      <c r="BZ2" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="CA2" s="22" t="s">
+      <c r="CA2" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="CB2" s="22" t="s">
+      <c r="CB2" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="CC2" s="10" t="s">
+      <c r="CC2" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="CD2" s="6" t="s">
+      <c r="CD2" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="CE2" s="10" t="s">
+      <c r="CE2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="CF2" s="6" t="s">
+      <c r="CF2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="CG2" s="5" t="s">
+      <c r="CG2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="CH2" s="5" t="s">
+      <c r="CH2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="CI2" s="5" t="s">
+      <c r="CI2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="CJ2" s="5" t="s">
+      <c r="CJ2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="CK2" s="26" t="s">
+      <c r="CK2" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="CL2" s="5" t="s">
+      <c r="CL2" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="CM2" s="5" t="s">
+      <c r="CM2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="CN2" s="5" t="s">
+      <c r="CN2" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="CO2" s="5" t="s">
+      <c r="CO2" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="CP2" s="5" t="s">
+      <c r="CP2" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="CQ2" s="5" t="s">
+      <c r="CQ2" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="CR2" s="5" t="s">
+      <c r="CR2" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="CS2" s="5" t="s">
+      <c r="CS2" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="CT2" s="12" t="s">
+      <c r="CT2" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="CU2" s="12" t="s">
+      <c r="CU2" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="CV2" s="12" t="s">
+      <c r="CV2" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="CW2" s="12" t="s">
+      <c r="CW2" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="CX2" s="12" t="s">
+      <c r="CX2" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="CY2" s="12" t="s">
+      <c r="CY2" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="CZ2" s="12" t="s">
+      <c r="CZ2" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="DA2" s="5" t="s">
+      <c r="DA2" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="DB2" s="5" t="s">
+      <c r="DB2" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="DC2" s="5" t="s">
+      <c r="DC2" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="DD2" s="5" t="s">
+      <c r="DD2" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="DE2" s="5" t="s">
+      <c r="DE2" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="DF2" s="12" t="s">
+      <c r="DF2" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="DG2" s="5" t="s">
+      <c r="DG2" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="DH2" s="40" t="s">
+      <c r="DH2" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="DI2" s="20" t="s">
+      <c r="DI2" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="DJ2" s="5" t="s">
+      <c r="DJ2" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="DK2" s="5" t="s">
+      <c r="DK2" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="DL2" s="12" t="s">
+      <c r="DL2" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="DM2" s="12" t="s">
+      <c r="DM2" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="DN2" s="12" t="s">
+      <c r="DN2" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="DO2" s="12" t="s">
+      <c r="DO2" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="DP2" s="12" t="s">
+      <c r="DP2" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="DQ2" s="12" t="s">
+      <c r="DQ2" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="DR2" s="12" t="s">
+      <c r="DR2" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="DS2" s="12" t="s">
+      <c r="DS2" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="DT2" s="5" t="s">
+      <c r="DT2" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="DU2" s="5" t="s">
+      <c r="DU2" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="DV2" s="5" t="s">
+      <c r="DV2" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="DW2" s="34" t="s">
+      <c r="DW2" s="18" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2463,7 +2466,7 @@
       <c r="AV3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AW3" s="9">
+      <c r="AW3" s="6">
         <v>1</v>
       </c>
       <c r="AX3" s="1">
@@ -2472,22 +2475,19 @@
       <c r="AY3" s="1">
         <v>3</v>
       </c>
-      <c r="AZ3" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BA3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC3" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BD3" s="17"/>
-      <c r="BE3" s="19"/>
-      <c r="BF3" s="19"/>
-      <c r="BG3" s="13" t="s">
+      <c r="AZ3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG3" s="1" t="s">
         <v>111</v>
       </c>
       <c r="BH3" s="1">
@@ -2508,7 +2508,7 @@
       <c r="BO3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="BQ3" s="9" t="s">
+      <c r="BQ3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="BR3" s="1" t="s">
@@ -2535,13 +2535,13 @@
       <c r="BY3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="CC3" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="CD3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="CE3" s="11" t="s">
+      <c r="CC3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE3" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2591,7 +2591,7 @@
       <c r="AV4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AW4" s="9">
+      <c r="AW4" s="6">
         <v>1</v>
       </c>
       <c r="AX4" s="1">
@@ -2600,22 +2600,19 @@
       <c r="AY4" s="1">
         <v>3</v>
       </c>
-      <c r="AZ4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BA4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BD4" s="17"/>
-      <c r="BE4" s="19"/>
-      <c r="BF4" s="19"/>
-      <c r="BG4" s="13" t="s">
+      <c r="AZ4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG4" s="1" t="s">
         <v>111</v>
       </c>
       <c r="BH4" s="1">
@@ -2636,7 +2633,7 @@
       <c r="BO4" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="BQ4" s="9" t="s">
+      <c r="BQ4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="BR4" s="1" t="s">
@@ -2663,13 +2660,13 @@
       <c r="BY4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="CC4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="CD4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="CE4" s="11" t="s">
+      <c r="CC4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE4" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2719,7 +2716,7 @@
       <c r="AV5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AW5" s="9">
+      <c r="AW5" s="6">
         <v>1</v>
       </c>
       <c r="AX5" s="1">
@@ -2728,22 +2725,19 @@
       <c r="AY5" s="1">
         <v>3</v>
       </c>
-      <c r="AZ5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BA5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BD5" s="17"/>
-      <c r="BE5" s="19"/>
-      <c r="BF5" s="19"/>
-      <c r="BG5" s="13" t="s">
+      <c r="AZ5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG5" s="1" t="s">
         <v>111</v>
       </c>
       <c r="BH5" s="1">
@@ -2764,7 +2758,7 @@
       <c r="BO5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="BQ5" s="9" t="s">
+      <c r="BQ5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="BR5" s="1" t="s">
@@ -2791,13 +2785,13 @@
       <c r="BY5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="CC5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="CD5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="CE5" s="11" t="s">
+      <c r="CC5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE5" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2847,7 +2841,7 @@
       <c r="AV6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AW6" s="9">
+      <c r="AW6" s="6">
         <v>1</v>
       </c>
       <c r="AX6" s="1">
@@ -2856,22 +2850,19 @@
       <c r="AY6" s="1">
         <v>3</v>
       </c>
-      <c r="AZ6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BA6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BD6" s="17"/>
-      <c r="BE6" s="19"/>
-      <c r="BF6" s="19"/>
-      <c r="BG6" s="13" t="s">
+      <c r="AZ6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG6" s="1" t="s">
         <v>111</v>
       </c>
       <c r="BH6" s="1">
@@ -2892,7 +2883,7 @@
       <c r="BO6" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="BQ6" s="9" t="s">
+      <c r="BQ6" s="6" t="s">
         <v>2</v>
       </c>
       <c r="BR6" s="1" t="s">
@@ -2919,13 +2910,13 @@
       <c r="BY6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="CC6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="CD6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="CE6" s="11" t="s">
+      <c r="CC6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE6" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2975,7 +2966,7 @@
       <c r="AV7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AW7" s="9">
+      <c r="AW7" s="6">
         <v>4</v>
       </c>
       <c r="AX7" s="1">
@@ -2984,29 +2975,24 @@
       <c r="AY7" s="1">
         <v>6</v>
       </c>
-      <c r="AZ7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BA7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BD7" s="17"/>
-      <c r="BE7" s="19"/>
-      <c r="BF7" s="19"/>
-      <c r="BG7" s="13" t="s">
+      <c r="AZ7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG7" s="1" t="s">
         <v>114</v>
       </c>
       <c r="BH7" s="1">
         <v>1</v>
       </c>
-      <c r="BI7" s="3"/>
-      <c r="BJ7" s="3"/>
       <c r="BK7" s="1" t="s">
         <v>21</v>
       </c>
@@ -3022,8 +3008,8 @@
       <c r="BO7" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="BP7" s="30"/>
-      <c r="BQ7" s="9" t="s">
+      <c r="BP7" s="14"/>
+      <c r="BQ7" s="6" t="s">
         <v>2</v>
       </c>
       <c r="BR7" s="1" t="s">
@@ -3050,13 +3036,13 @@
       <c r="BY7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="CC7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="CD7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="CE7" s="11" t="s">
+      <c r="CC7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE7" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3106,7 +3092,7 @@
       <c r="AV8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AW8" s="9" t="s">
+      <c r="AW8" s="6" t="s">
         <v>2</v>
       </c>
       <c r="AX8" s="1" t="s">
@@ -3115,29 +3101,24 @@
       <c r="AY8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AZ8" s="17" t="s">
+      <c r="AZ8" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="BA8" s="3" t="s">
+      <c r="BA8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BB8" s="3" t="s">
+      <c r="BB8" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="BC8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BD8" s="17"/>
-      <c r="BE8" s="19"/>
-      <c r="BF8" s="19"/>
-      <c r="BG8" s="14" t="s">
+      <c r="BC8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG8" s="2" t="s">
         <v>112</v>
       </c>
       <c r="BH8" s="2">
         <v>2</v>
       </c>
-      <c r="BI8" s="3"/>
-      <c r="BJ8" s="3"/>
       <c r="BK8" s="1" t="s">
         <v>27</v>
       </c>
@@ -3153,32 +3134,23 @@
       <c r="BO8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="BP8" s="30"/>
-      <c r="BQ8" s="17" t="s">
+      <c r="BP8" s="14"/>
+      <c r="BQ8" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="BR8" s="3" t="s">
+      <c r="BR8" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="BS8" s="3" t="s">
+      <c r="BS8" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="BT8" s="3"/>
-      <c r="BU8" s="3"/>
-      <c r="BV8" s="3"/>
-      <c r="BW8" s="3"/>
-      <c r="BX8" s="3"/>
-      <c r="BY8" s="3"/>
-      <c r="BZ8" s="17"/>
-      <c r="CA8" s="15"/>
-      <c r="CB8" s="15"/>
-      <c r="CC8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="CD8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="CE8" s="17" t="s">
+      <c r="CC8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE8" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3228,7 +3200,7 @@
       <c r="AV9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AW9" s="9" t="s">
+      <c r="AW9" s="6" t="s">
         <v>2</v>
       </c>
       <c r="AX9" s="1" t="s">
@@ -3237,29 +3209,24 @@
       <c r="AY9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AZ9" s="17" t="s">
+      <c r="AZ9" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="BA9" s="3" t="s">
+      <c r="BA9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BB9" s="3" t="s">
+      <c r="BB9" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="BC9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BD9" s="17"/>
-      <c r="BE9" s="19"/>
-      <c r="BF9" s="19"/>
-      <c r="BG9" s="14" t="s">
+      <c r="BC9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG9" s="2" t="s">
         <v>113</v>
       </c>
       <c r="BH9" s="2">
         <v>2</v>
       </c>
-      <c r="BI9" s="3"/>
-      <c r="BJ9" s="3"/>
       <c r="BK9" s="1" t="s">
         <v>27</v>
       </c>
@@ -3275,38 +3242,32 @@
       <c r="BO9" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="BP9" s="30"/>
-      <c r="BQ9" s="17" t="s">
+      <c r="BP9" s="14"/>
+      <c r="BQ9" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="BR9" s="3" t="s">
+      <c r="BR9" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BS9" s="3" t="s">
+      <c r="BS9" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BT9" s="3"/>
-      <c r="BU9" s="3"/>
-      <c r="BV9" s="3"/>
-      <c r="BW9" s="3"/>
-      <c r="BX9" s="3"/>
-      <c r="BY9" s="3"/>
-      <c r="BZ9" s="17" t="s">
+      <c r="BZ9" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="CA9" s="15" t="s">
+      <c r="CA9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="CB9" s="15" t="s">
+      <c r="CB9" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="CC9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="CD9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="CE9" s="17" t="s">
+      <c r="CC9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE9" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3356,7 +3317,7 @@
       <c r="AV10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AW10" s="9" t="s">
+      <c r="AW10" s="6" t="s">
         <v>2</v>
       </c>
       <c r="AX10" s="1" t="s">
@@ -3365,29 +3326,24 @@
       <c r="AY10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AZ10" s="17" t="s">
+      <c r="AZ10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="BA10" s="3" t="s">
+      <c r="BA10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BB10" s="3" t="s">
+      <c r="BB10" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="BC10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BD10" s="17"/>
-      <c r="BE10" s="19"/>
-      <c r="BF10" s="19"/>
-      <c r="BG10" s="13" t="s">
+      <c r="BC10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG10" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BH10" s="2">
         <v>2</v>
       </c>
-      <c r="BI10" s="3"/>
-      <c r="BJ10" s="3"/>
       <c r="BK10" s="1" t="s">
         <v>27</v>
       </c>
@@ -3403,38 +3359,32 @@
       <c r="BO10" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="BP10" s="30"/>
-      <c r="BQ10" s="17" t="s">
+      <c r="BP10" s="14"/>
+      <c r="BQ10" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="BR10" s="3" t="s">
+      <c r="BR10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BS10" s="3" t="s">
+      <c r="BS10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BT10" s="3"/>
-      <c r="BU10" s="3"/>
-      <c r="BV10" s="3"/>
-      <c r="BW10" s="3"/>
-      <c r="BX10" s="3"/>
-      <c r="BY10" s="3"/>
-      <c r="BZ10" s="17" t="s">
+      <c r="BZ10" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="CA10" s="15" t="s">
+      <c r="CA10" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="CB10" s="15" t="s">
+      <c r="CB10" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="CC10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="CD10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="CE10" s="17" t="s">
+      <c r="CC10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE10" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3484,7 +3434,7 @@
       <c r="AV11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AW11" s="9" t="s">
+      <c r="AW11" s="6" t="s">
         <v>2</v>
       </c>
       <c r="AX11" s="1" t="s">
@@ -3493,29 +3443,24 @@
       <c r="AY11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AZ11" s="17" t="s">
+      <c r="AZ11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="BA11" s="3" t="s">
+      <c r="BA11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BB11" s="3" t="s">
+      <c r="BB11" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="BC11" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BD11" s="17"/>
-      <c r="BE11" s="19"/>
-      <c r="BF11" s="19"/>
-      <c r="BG11" s="13" t="s">
+      <c r="BC11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG11" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BH11" s="2">
         <v>2</v>
       </c>
-      <c r="BI11" s="3"/>
-      <c r="BJ11" s="3"/>
       <c r="BK11" s="1" t="s">
         <v>27</v>
       </c>
@@ -3531,38 +3476,32 @@
       <c r="BO11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="BP11" s="30"/>
-      <c r="BQ11" s="17" t="s">
+      <c r="BP11" s="14"/>
+      <c r="BQ11" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="BR11" s="3" t="s">
+      <c r="BR11" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BS11" s="3" t="s">
+      <c r="BS11" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BT11" s="3"/>
-      <c r="BU11" s="3"/>
-      <c r="BV11" s="3"/>
-      <c r="BW11" s="3"/>
-      <c r="BX11" s="3"/>
-      <c r="BY11" s="3"/>
-      <c r="BZ11" s="17" t="s">
+      <c r="BZ11" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="CA11" s="15" t="s">
+      <c r="CA11" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="CB11" s="15" t="s">
+      <c r="CB11" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="CC11" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="CD11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="CE11" s="17" t="s">
+      <c r="CC11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE11" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3612,7 +3551,7 @@
       <c r="AV12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AW12" s="9" t="s">
+      <c r="AW12" s="6" t="s">
         <v>2</v>
       </c>
       <c r="AX12" s="1" t="s">
@@ -3621,29 +3560,24 @@
       <c r="AY12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AZ12" s="17" t="s">
+      <c r="AZ12" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="BA12" s="3" t="s">
+      <c r="BA12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BB12" s="3" t="s">
+      <c r="BB12" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="BC12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BD12" s="17"/>
-      <c r="BE12" s="19"/>
-      <c r="BF12" s="19"/>
-      <c r="BG12" s="13" t="s">
+      <c r="BC12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG12" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BH12" s="2">
         <v>2</v>
       </c>
-      <c r="BI12" s="3"/>
-      <c r="BJ12" s="3"/>
       <c r="BK12" s="1" t="s">
         <v>27</v>
       </c>
@@ -3659,38 +3593,32 @@
       <c r="BO12" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="BP12" s="30"/>
-      <c r="BQ12" s="17" t="s">
+      <c r="BP12" s="14"/>
+      <c r="BQ12" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="BR12" s="3" t="s">
+      <c r="BR12" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BS12" s="3" t="s">
+      <c r="BS12" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BT12" s="3"/>
-      <c r="BU12" s="3"/>
-      <c r="BV12" s="3"/>
-      <c r="BW12" s="3"/>
-      <c r="BX12" s="3"/>
-      <c r="BY12" s="3"/>
-      <c r="BZ12" s="17" t="s">
+      <c r="BZ12" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="CA12" s="15" t="s">
+      <c r="CA12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="CB12" s="15" t="s">
+      <c r="CB12" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="CC12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="CD12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="CE12" s="17" t="s">
+      <c r="CC12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE12" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3740,7 +3668,7 @@
       <c r="AV13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AW13" s="9" t="s">
+      <c r="AW13" s="6" t="s">
         <v>2</v>
       </c>
       <c r="AX13" s="1" t="s">
@@ -3749,29 +3677,24 @@
       <c r="AY13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AZ13" s="17" t="s">
+      <c r="AZ13" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="BA13" s="3" t="s">
+      <c r="BA13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BB13" s="3" t="s">
+      <c r="BB13" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="BC13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BD13" s="17"/>
-      <c r="BE13" s="19"/>
-      <c r="BF13" s="19"/>
-      <c r="BG13" s="13" t="s">
+      <c r="BC13" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG13" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BH13" s="2">
         <v>2</v>
       </c>
-      <c r="BI13" s="3"/>
-      <c r="BJ13" s="3"/>
       <c r="BK13" s="1" t="s">
         <v>27</v>
       </c>
@@ -3787,38 +3710,32 @@
       <c r="BO13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="BP13" s="30"/>
-      <c r="BQ13" s="17" t="s">
+      <c r="BP13" s="14"/>
+      <c r="BQ13" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="BR13" s="3" t="s">
+      <c r="BR13" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BS13" s="3" t="s">
+      <c r="BS13" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BT13" s="3"/>
-      <c r="BU13" s="3"/>
-      <c r="BV13" s="3"/>
-      <c r="BW13" s="3"/>
-      <c r="BX13" s="3"/>
-      <c r="BY13" s="3"/>
-      <c r="BZ13" s="17" t="s">
+      <c r="BZ13" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="CA13" s="15" t="s">
+      <c r="CA13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="CB13" s="15" t="s">
+      <c r="CB13" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="CC13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="CD13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="CE13" s="17" t="s">
+      <c r="CC13" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE13" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3868,7 +3785,7 @@
       <c r="AV14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AW14" s="9" t="s">
+      <c r="AW14" s="6" t="s">
         <v>2</v>
       </c>
       <c r="AX14" s="1" t="s">
@@ -3877,29 +3794,24 @@
       <c r="AY14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AZ14" s="17" t="s">
+      <c r="AZ14" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="BA14" s="3" t="s">
+      <c r="BA14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BB14" s="3" t="s">
+      <c r="BB14" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="BC14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BD14" s="17"/>
-      <c r="BE14" s="19"/>
-      <c r="BF14" s="19"/>
-      <c r="BG14" s="13" t="s">
+      <c r="BC14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG14" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BH14" s="2">
         <v>2</v>
       </c>
-      <c r="BI14" s="3"/>
-      <c r="BJ14" s="3"/>
       <c r="BK14" s="1" t="s">
         <v>27</v>
       </c>
@@ -3915,38 +3827,32 @@
       <c r="BO14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="BP14" s="30"/>
-      <c r="BQ14" s="17" t="s">
+      <c r="BP14" s="14"/>
+      <c r="BQ14" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="BR14" s="3" t="s">
+      <c r="BR14" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BS14" s="3" t="s">
+      <c r="BS14" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BT14" s="3"/>
-      <c r="BU14" s="3"/>
-      <c r="BV14" s="3"/>
-      <c r="BW14" s="3"/>
-      <c r="BX14" s="3"/>
-      <c r="BY14" s="3"/>
-      <c r="BZ14" s="17" t="s">
+      <c r="BZ14" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="CA14" s="15" t="s">
+      <c r="CA14" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="CB14" s="15" t="s">
+      <c r="CB14" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="CC14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="CD14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="CE14" s="17" t="s">
+      <c r="CC14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE14" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3996,7 +3902,7 @@
       <c r="AV15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AW15" s="9" t="s">
+      <c r="AW15" s="6" t="s">
         <v>2</v>
       </c>
       <c r="AX15" s="1" t="s">
@@ -4005,29 +3911,24 @@
       <c r="AY15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AZ15" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BA15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC15" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BD15" s="17"/>
-      <c r="BE15" s="19"/>
-      <c r="BF15" s="19"/>
-      <c r="BG15" s="14" t="s">
+      <c r="AZ15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG15" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="BH15" s="3">
-        <v>2</v>
-      </c>
-      <c r="BI15" s="3"/>
-      <c r="BJ15" s="3"/>
+      <c r="BH15" s="1">
+        <v>2</v>
+      </c>
       <c r="BK15" s="2" t="s">
         <v>2</v>
       </c>
@@ -4040,47 +3941,44 @@
       <c r="BN15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="BO15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BP15" s="30"/>
-      <c r="BQ15" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BR15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BS15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BT15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BU15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BV15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BW15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BX15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BY15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BZ15" s="17"/>
-      <c r="CA15" s="15"/>
-      <c r="CB15" s="15"/>
-      <c r="CC15" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="CD15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="CE15" s="17" t="s">
+      <c r="BO15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP15" s="14"/>
+      <c r="BQ15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BR15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BT15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BU15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BV15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BW15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BX15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CC15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE15" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4127,10 +4025,10 @@
       <c r="AU16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AV16" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW16" s="9" t="s">
+      <c r="AV16" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW16" s="6" t="s">
         <v>2</v>
       </c>
       <c r="AX16" s="1" t="s">
@@ -4139,29 +4037,24 @@
       <c r="AY16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AZ16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BA16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC16" s="17" t="s">
+      <c r="AZ16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC16" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="BD16" s="17"/>
-      <c r="BE16" s="19"/>
-      <c r="BF16" s="19"/>
-      <c r="BG16" s="14" t="s">
+      <c r="BG16" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="BH16" s="3">
+      <c r="BH16" s="1">
         <v>1</v>
       </c>
-      <c r="BI16" s="3"/>
-      <c r="BJ16" s="3"/>
       <c r="BK16" s="2" t="s">
         <v>2</v>
       </c>
@@ -4174,50 +4067,46 @@
       <c r="BN16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="BO16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BP16" s="30"/>
-      <c r="BQ16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BR16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BS16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BT16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BU16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BV16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BW16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BX16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BY16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BZ16" s="17"/>
-      <c r="CA16" s="15"/>
-      <c r="CB16" s="15"/>
-      <c r="CC16" s="17" t="s">
+      <c r="BO16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP16" s="14"/>
+      <c r="BQ16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BR16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BT16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BU16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BV16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BW16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BX16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CC16" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="CD16" s="3">
+      <c r="CD16" s="1">
         <v>5000</v>
       </c>
-      <c r="CE16" s="17" t="s">
+      <c r="CE16" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="CF16" s="3"/>
     </row>
     <row r="17" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -4262,10 +4151,10 @@
       <c r="AU17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AV17" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW17" s="9" t="s">
+      <c r="AV17" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW17" s="6" t="s">
         <v>2</v>
       </c>
       <c r="AX17" s="1" t="s">
@@ -4274,29 +4163,24 @@
       <c r="AY17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AZ17" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BA17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC17" s="17" t="s">
+      <c r="AZ17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC17" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="BD17" s="17"/>
-      <c r="BE17" s="19"/>
-      <c r="BF17" s="19"/>
-      <c r="BG17" s="14" t="s">
+      <c r="BG17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="BH17" s="3">
+      <c r="BH17" s="1">
         <v>1</v>
       </c>
-      <c r="BI17" s="3"/>
-      <c r="BJ17" s="3"/>
       <c r="BK17" s="2" t="s">
         <v>2</v>
       </c>
@@ -4309,47 +4193,43 @@
       <c r="BN17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="BO17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BP17" s="3"/>
-      <c r="BQ17" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BR17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BS17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BT17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BU17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BV17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BW17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BX17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BY17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BZ17" s="17"/>
-      <c r="CA17" s="15"/>
-      <c r="CB17" s="15"/>
-      <c r="CC17" s="17" t="s">
+      <c r="BO17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BQ17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BR17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BT17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BU17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BV17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BW17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BX17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="CC17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="CD17" s="3">
+      <c r="CD17" s="1">
         <v>4000</v>
       </c>
-      <c r="CE17" s="17" t="s">
+      <c r="CE17" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4387,21 +4267,6 @@
       <c r="AN18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="BH18" s="3"/>
-      <c r="BI18" s="3"/>
-      <c r="BJ18" s="3"/>
-      <c r="BQ18" s="17"/>
-      <c r="BR18" s="3"/>
-      <c r="BS18" s="3"/>
-      <c r="BT18" s="3"/>
-      <c r="BU18" s="3"/>
-      <c r="BV18" s="3"/>
-      <c r="BW18" s="3"/>
-      <c r="BX18" s="3"/>
-      <c r="BY18" s="3"/>
-      <c r="BZ18" s="17"/>
-      <c r="CA18" s="15"/>
-      <c r="CB18" s="15"/>
     </row>
     <row r="19" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -4437,21 +4302,6 @@
       <c r="AN19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="BH19" s="3"/>
-      <c r="BI19" s="3"/>
-      <c r="BJ19" s="3"/>
-      <c r="BQ19" s="17"/>
-      <c r="BR19" s="3"/>
-      <c r="BS19" s="3"/>
-      <c r="BT19" s="3"/>
-      <c r="BU19" s="3"/>
-      <c r="BV19" s="3"/>
-      <c r="BW19" s="3"/>
-      <c r="BX19" s="3"/>
-      <c r="BY19" s="3"/>
-      <c r="BZ19" s="17"/>
-      <c r="CA19" s="15"/>
-      <c r="CB19" s="15"/>
     </row>
     <row r="20" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">

</xml_diff>